<commit_message>
Change to languages and classification
</commit_message>
<xml_diff>
--- a/app-conf/data/datarep/species/templates/Classifications.xlsx
+++ b/app-conf/data/datarep/species/templates/Classifications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Froese, R. and D. Pauly. Editors. 2011.FishBase.World Wide Web electronic publication.&lt;a href='http://www.fishbase.org/' target='_blank' &gt;www.fishbase.org, version (10/2011).&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Flora of Bhutan Taxonomy Hierarchy</t>
   </si>
   <si>
     <t>Eflora Taxonomy Hierarchy</t>
@@ -95,7 +98,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -130,6 +133,12 @@
       <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
       <color rgb="00000000"/>
       <sz val="10"/>
     </font>
@@ -176,7 +185,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -188,6 +197,9 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -207,19 +219,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.0117647058823"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="68.1725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.3372549019608"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.8313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.1372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="68.4588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.9882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.93333333333333"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -250,7 +262,6 @@
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="0"/>
       <c r="E3" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
@@ -260,7 +271,6 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
@@ -269,7 +279,6 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
@@ -278,7 +287,14 @@
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -308,63 +324,63 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.0470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.93333333333333"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="10">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -390,7 +406,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.93333333333333"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added additional classification, and loading taxon names
</commit_message>
<xml_diff>
--- a/app-conf/data/datarep/species/templates/Classifications.xlsx
+++ b/app-conf/data/datarep/species/templates/Classifications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,12 @@
     <t>Flora of Bhutan Taxonomy Hierarchy</t>
   </si>
   <si>
+    <t>eBird Taxonomy Hierarchy (2010)</t>
+  </si>
+  <si>
+    <t>Catalogue of Life Taxonomy Hierarchy</t>
+  </si>
+  <si>
     <t>Eflora Taxonomy Hierarchy</t>
   </si>
   <si>
@@ -79,16 +85,10 @@
     <t>Clements 6th edition Taxonomy Hierarchy (2009)</t>
   </si>
   <si>
-    <t>eBird Taxonomy Hierarchy (2010)</t>
-  </si>
-  <si>
     <t>OBC Taxonomy Hierarchy (2001)</t>
   </si>
   <si>
     <t>Flowers of India Taxonomy Hierarchy</t>
-  </si>
-  <si>
-    <t>Catalogue of Life Taxonomy Hierarchy</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -135,6 +135,13 @@
       <b val="true"/>
       <color rgb="00000000"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial Narrow"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +186,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -193,6 +200,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -210,18 +218,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="D7"/>
+      <selection activeCell="B13" activeCellId="0" pane="topLeft" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="96.9490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.6509803921569"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.3882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="97.3529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.8078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.3176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -279,12 +288,26 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -314,62 +337,63 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2117647058823"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.3764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -394,6 +418,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>